<commit_message>
fix isTrialBalanceBalanced method in AbstractTrialBalance
</commit_message>
<xml_diff>
--- a/src/input_trial_balances/TESTUS04.xlsx
+++ b/src/input_trial_balances/TESTUS04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmuther/Dev/Personal/Consolidation_Tool_Java/src/input_trial_balances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5B0EA9-90D6-1545-B038-0A184413F02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F9129C-E737-FF42-9A26-48EA7125CBE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="1000" windowWidth="27160" windowHeight="16440" xr2:uid="{7D95F7F2-E310-FE42-B6BB-709D674CF68E}"/>
   </bookViews>
@@ -516,7 +516,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C3:C36"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,7 +625,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="2">
-        <v>-33000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -746,7 +746,7 @@
         <v>22</v>
       </c>
       <c r="C20" s="2">
-        <v>1000</v>
+        <v>-33000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>